<commit_message>
initial changes, adding config.R
</commit_message>
<xml_diff>
--- a/Data Prep/VERSPM File Summary Tracker.xlsx
+++ b/Data Prep/VERSPM File Summary Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eric.englin\Desktop\Github Volpe\VE-Tools\Data Prep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70736D16-BFDF-4A6D-B979-BD494AF4EDC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC280898-5F12-480C-A04F-ED3107B50B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1770" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -3310,6 +3310,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -3349,9 +3352,6 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3655,8 +3655,8 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3769,7 +3769,7 @@
       <c r="Z3" s="16"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="147"/>
+      <c r="A4" s="124"/>
       <c r="B4" s="18" t="s">
         <v>13</v>
       </c>
@@ -3819,7 +3819,7 @@
       <c r="Z4" s="23"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="147"/>
+      <c r="A5" s="124"/>
       <c r="B5" s="18" t="s">
         <v>23</v>
       </c>
@@ -3869,7 +3869,7 @@
       <c r="Z5" s="23"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="147"/>
+      <c r="A6" s="124"/>
       <c r="B6" s="18" t="s">
         <v>23</v>
       </c>
@@ -3915,7 +3915,7 @@
       <c r="Z6" s="23"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="147"/>
+      <c r="A7" s="124"/>
       <c r="B7" s="18" t="s">
         <v>36</v>
       </c>
@@ -3965,7 +3965,7 @@
       <c r="Z7" s="23"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="147"/>
+      <c r="A8" s="124"/>
       <c r="B8" s="18" t="s">
         <v>43</v>
       </c>
@@ -4011,7 +4011,7 @@
       <c r="Z8" s="23"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="147"/>
+      <c r="A9" s="124"/>
       <c r="B9" s="18" t="s">
         <v>51</v>
       </c>
@@ -4057,7 +4057,7 @@
       <c r="Z9" s="23"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="147"/>
+      <c r="A10" s="124"/>
       <c r="B10" s="18" t="s">
         <v>51</v>
       </c>
@@ -4103,7 +4103,7 @@
       <c r="Z10" s="23"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="147"/>
+      <c r="A11" s="124"/>
       <c r="B11" s="18" t="s">
         <v>13</v>
       </c>
@@ -4153,7 +4153,7 @@
       <c r="Z11" s="23"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="147"/>
+      <c r="A12" s="124"/>
       <c r="B12" s="18" t="s">
         <v>43</v>
       </c>
@@ -4199,7 +4199,7 @@
       <c r="Z12" s="23"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="147"/>
+      <c r="A13" s="124"/>
       <c r="B13" s="18" t="s">
         <v>13</v>
       </c>
@@ -4249,7 +4249,7 @@
       <c r="Z13" s="23"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="147"/>
+      <c r="A14" s="124"/>
       <c r="B14" s="18" t="s">
         <v>13</v>
       </c>
@@ -4297,7 +4297,7 @@
       <c r="Z14" s="23"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="147"/>
+      <c r="A15" s="124"/>
       <c r="B15" s="18" t="s">
         <v>43</v>
       </c>
@@ -4343,7 +4343,7 @@
       <c r="Z15" s="23"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="147"/>
+      <c r="A16" s="124"/>
       <c r="B16" s="18" t="s">
         <v>51</v>
       </c>
@@ -4391,7 +4391,7 @@
       <c r="Z16" s="23"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="147"/>
+      <c r="A17" s="124"/>
       <c r="B17" s="18" t="s">
         <v>13</v>
       </c>
@@ -4441,7 +4441,7 @@
       <c r="Z17" s="23"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="147"/>
+      <c r="A18" s="124"/>
       <c r="B18" s="18" t="s">
         <v>43</v>
       </c>
@@ -4487,7 +4487,7 @@
       <c r="Z18" s="23"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="147"/>
+      <c r="A19" s="124"/>
       <c r="B19" s="18" t="s">
         <v>89</v>
       </c>
@@ -4535,7 +4535,7 @@
       <c r="Z19" s="23"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="147"/>
+      <c r="A20" s="124"/>
       <c r="B20" s="18" t="s">
         <v>43</v>
       </c>
@@ -4585,7 +4585,7 @@
       <c r="Z20" s="23"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="147"/>
+      <c r="A21" s="124"/>
       <c r="B21" s="18" t="s">
         <v>36</v>
       </c>
@@ -4633,7 +4633,7 @@
       <c r="Z21" s="23"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="147"/>
+      <c r="A22" s="124"/>
       <c r="B22" s="18" t="s">
         <v>36</v>
       </c>
@@ -4683,7 +4683,7 @@
       <c r="Z22" s="23"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="147"/>
+      <c r="A23" s="124"/>
       <c r="B23" s="18" t="s">
         <v>51</v>
       </c>
@@ -4731,7 +4731,7 @@
       <c r="Z23" s="23"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="147"/>
+      <c r="A24" s="124"/>
       <c r="B24" s="18" t="s">
         <v>113</v>
       </c>
@@ -4777,7 +4777,7 @@
       <c r="Z24" s="23"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="147"/>
+      <c r="A25" s="124"/>
       <c r="B25" s="18" t="s">
         <v>113</v>
       </c>
@@ -4823,7 +4823,7 @@
       <c r="Z25" s="23"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="147"/>
+      <c r="A26" s="124"/>
       <c r="B26" s="18" t="s">
         <v>120</v>
       </c>
@@ -4871,7 +4871,7 @@
       <c r="Z26" s="23"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="147"/>
+      <c r="A27" s="124"/>
       <c r="B27" s="18" t="s">
         <v>113</v>
       </c>
@@ -4919,7 +4919,7 @@
       <c r="Z27" s="23"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="147"/>
+      <c r="A28" s="124"/>
       <c r="B28" s="18" t="s">
         <v>120</v>
       </c>
@@ -4965,7 +4965,7 @@
       <c r="Z28" s="23"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="147"/>
+      <c r="A29" s="124"/>
       <c r="B29" s="18" t="s">
         <v>113</v>
       </c>
@@ -5013,7 +5013,7 @@
       <c r="Z29" s="23"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="147"/>
+      <c r="A30" s="124"/>
       <c r="B30" s="18" t="s">
         <v>113</v>
       </c>
@@ -5059,7 +5059,7 @@
       <c r="Z30" s="23"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="147"/>
+      <c r="A31" s="124"/>
       <c r="B31" s="18" t="s">
         <v>142</v>
       </c>
@@ -5107,7 +5107,7 @@
       <c r="Z31" s="23"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="147"/>
+      <c r="A32" s="124"/>
       <c r="B32" s="18" t="s">
         <v>113</v>
       </c>
@@ -5153,7 +5153,7 @@
       <c r="Z32" s="23"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="147"/>
+      <c r="A33" s="124"/>
       <c r="B33" s="18" t="s">
         <v>113</v>
       </c>
@@ -5201,7 +5201,7 @@
       <c r="Z33" s="23"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="147"/>
+      <c r="A34" s="124"/>
       <c r="B34" s="18" t="s">
         <v>113</v>
       </c>
@@ -5251,7 +5251,7 @@
       <c r="Z34" s="23"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="147"/>
+      <c r="A35" s="124"/>
       <c r="B35" s="18" t="s">
         <v>113</v>
       </c>
@@ -5297,7 +5297,7 @@
       <c r="Z35" s="23"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="147"/>
+      <c r="A36" s="124"/>
       <c r="B36" s="18" t="s">
         <v>161</v>
       </c>
@@ -5347,7 +5347,7 @@
       <c r="Z36" s="23"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="147"/>
+      <c r="A37" s="124"/>
       <c r="B37" s="18" t="s">
         <v>161</v>
       </c>
@@ -5393,7 +5393,7 @@
       <c r="Z37" s="23"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="147"/>
+      <c r="A38" s="124"/>
       <c r="B38" s="18" t="s">
         <v>36</v>
       </c>
@@ -5441,7 +5441,7 @@
       <c r="Z38" s="23"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="147"/>
+      <c r="A39" s="124"/>
       <c r="B39" s="18" t="s">
         <v>51</v>
       </c>
@@ -5489,7 +5489,7 @@
       <c r="Z39" s="23"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="147"/>
+      <c r="A40" s="124"/>
       <c r="B40" s="18" t="s">
         <v>36</v>
       </c>
@@ -5537,7 +5537,7 @@
       <c r="Z40" s="23"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="147"/>
+      <c r="A41" s="124"/>
       <c r="B41" s="18" t="s">
         <v>51</v>
       </c>
@@ -5585,7 +5585,7 @@
       <c r="Z41" s="23"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="147"/>
+      <c r="A42" s="124"/>
       <c r="B42" s="18" t="s">
         <v>36</v>
       </c>
@@ -5633,7 +5633,7 @@
       <c r="Z42" s="23"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="147"/>
+      <c r="A43" s="124"/>
       <c r="B43" s="18" t="s">
         <v>142</v>
       </c>
@@ -5679,7 +5679,7 @@
       <c r="Z43" s="23"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="147"/>
+      <c r="A44" s="124"/>
       <c r="B44" s="18" t="s">
         <v>51</v>
       </c>
@@ -5727,7 +5727,7 @@
       <c r="Z44" s="23"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="147"/>
+      <c r="A45" s="124"/>
       <c r="B45" s="18" t="s">
         <v>36</v>
       </c>
@@ -5773,7 +5773,7 @@
       <c r="Z45" s="23"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="147"/>
+      <c r="A46" s="124"/>
       <c r="B46" s="18" t="s">
         <v>51</v>
       </c>
@@ -5821,7 +5821,7 @@
       <c r="Z46" s="23"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="147"/>
+      <c r="A47" s="124"/>
       <c r="B47" s="18" t="s">
         <v>51</v>
       </c>
@@ -5869,7 +5869,7 @@
       <c r="Z47" s="23"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="147"/>
+      <c r="A48" s="124"/>
       <c r="B48" s="18" t="s">
         <v>36</v>
       </c>
@@ -5919,7 +5919,7 @@
       <c r="Z48" s="23"/>
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="147"/>
+      <c r="A49" s="124"/>
       <c r="B49" s="18" t="s">
         <v>23</v>
       </c>
@@ -5965,7 +5965,7 @@
       <c r="Z49" s="23"/>
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="147"/>
+      <c r="A50" s="124"/>
       <c r="B50" s="18" t="s">
         <v>23</v>
       </c>
@@ -6011,7 +6011,7 @@
       <c r="Z50" s="23"/>
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="147"/>
+      <c r="A51" s="124"/>
       <c r="B51" s="18" t="s">
         <v>23</v>
       </c>
@@ -6057,7 +6057,7 @@
       <c r="Z51" s="23"/>
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="147"/>
+      <c r="A52" s="124"/>
       <c r="B52" s="18" t="s">
         <v>23</v>
       </c>
@@ -6103,7 +6103,7 @@
       <c r="Z52" s="23"/>
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="147"/>
+      <c r="A53" s="124"/>
       <c r="B53" s="18" t="s">
         <v>142</v>
       </c>
@@ -6151,7 +6151,7 @@
       <c r="Z53" s="23"/>
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="147"/>
+      <c r="A54" s="124"/>
       <c r="B54" s="18" t="s">
         <v>51</v>
       </c>
@@ -6199,7 +6199,7 @@
       <c r="Z54" s="23"/>
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="147"/>
+      <c r="A55" s="124"/>
       <c r="B55" s="18" t="s">
         <v>51</v>
       </c>
@@ -6245,7 +6245,7 @@
       <c r="Z55" s="23"/>
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="147"/>
+      <c r="A56" s="124"/>
       <c r="B56" s="18" t="s">
         <v>161</v>
       </c>
@@ -6295,7 +6295,7 @@
       <c r="Z56" s="23"/>
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="147"/>
+      <c r="A57" s="124"/>
       <c r="B57" s="18" t="s">
         <v>36</v>
       </c>
@@ -6345,7 +6345,7 @@
       <c r="Z57" s="23"/>
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="147"/>
+      <c r="A58" s="124"/>
       <c r="B58" s="18" t="s">
         <v>23</v>
       </c>
@@ -6393,7 +6393,7 @@
       <c r="Z58" s="23"/>
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="147"/>
+      <c r="A59" s="124"/>
       <c r="B59" s="18" t="s">
         <v>36</v>
       </c>
@@ -6441,7 +6441,7 @@
       <c r="Z59" s="23"/>
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="147"/>
+      <c r="A60" s="124"/>
       <c r="B60" s="18" t="s">
         <v>23</v>
       </c>
@@ -6491,7 +6491,7 @@
       <c r="Z60" s="23"/>
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="147"/>
+      <c r="A61" s="124"/>
       <c r="B61" s="18" t="s">
         <v>36</v>
       </c>
@@ -6541,7 +6541,7 @@
       <c r="Z61" s="23"/>
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="147"/>
+      <c r="A62" s="124"/>
       <c r="B62" s="18" t="s">
         <v>36</v>
       </c>
@@ -6591,7 +6591,7 @@
       <c r="Z62" s="23"/>
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="147"/>
+      <c r="A63" s="124"/>
       <c r="B63" s="18" t="s">
         <v>23</v>
       </c>
@@ -6641,7 +6641,7 @@
       <c r="Z63" s="23"/>
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="147"/>
+      <c r="A64" s="124"/>
       <c r="B64" s="18" t="s">
         <v>36</v>
       </c>
@@ -6691,7 +6691,7 @@
       <c r="Z64" s="23"/>
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="147"/>
+      <c r="A65" s="124"/>
       <c r="B65" s="18" t="s">
         <v>13</v>
       </c>
@@ -6741,7 +6741,7 @@
       <c r="Z65" s="23"/>
     </row>
     <row r="66" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="147"/>
+      <c r="A66" s="124"/>
       <c r="B66" s="18" t="s">
         <v>23</v>
       </c>
@@ -6791,7 +6791,7 @@
       <c r="Z66" s="23"/>
     </row>
     <row r="67" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="147"/>
+      <c r="A67" s="124"/>
       <c r="B67" s="18" t="s">
         <v>36</v>
       </c>
@@ -6839,7 +6839,7 @@
       <c r="Z67" s="23"/>
     </row>
     <row r="68" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="147"/>
+      <c r="A68" s="124"/>
       <c r="B68" s="18" t="s">
         <v>36</v>
       </c>
@@ -29729,15 +29729,15 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C2" s="136" t="s">
+      <c r="C2" s="137" t="s">
         <v>387</v>
       </c>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="139"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="23"/>
@@ -29970,26 +29970,26 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B13" s="139" t="s">
+      <c r="B13" s="140" t="s">
         <v>409</v>
       </c>
-      <c r="C13" s="140"/>
-      <c r="D13" s="140"/>
-      <c r="E13" s="140"/>
-      <c r="F13" s="140"/>
-      <c r="G13" s="140"/>
-      <c r="H13" s="140"/>
-      <c r="I13" s="140"/>
+      <c r="C13" s="141"/>
+      <c r="D13" s="141"/>
+      <c r="E13" s="141"/>
+      <c r="F13" s="141"/>
+      <c r="G13" s="141"/>
+      <c r="H13" s="141"/>
+      <c r="I13" s="141"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="141"/>
-      <c r="C14" s="141"/>
-      <c r="D14" s="141"/>
-      <c r="E14" s="141"/>
-      <c r="F14" s="141"/>
-      <c r="G14" s="141"/>
-      <c r="H14" s="141"/>
-      <c r="I14" s="141"/>
+      <c r="B14" s="142"/>
+      <c r="C14" s="142"/>
+      <c r="D14" s="142"/>
+      <c r="E14" s="142"/>
+      <c r="F14" s="142"/>
+      <c r="G14" s="142"/>
+      <c r="H14" s="142"/>
+      <c r="I14" s="142"/>
     </row>
     <row r="15" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="C15" s="92" t="s">
@@ -30002,47 +30002,47 @@
       </c>
     </row>
     <row r="18" spans="1:26" ht="213" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="142" t="s">
+      <c r="A18" s="143" t="s">
         <v>412</v>
       </c>
-      <c r="B18" s="141"/>
-      <c r="C18" s="141"/>
-      <c r="D18" s="141"/>
-      <c r="E18" s="141"/>
-      <c r="F18" s="141"/>
-      <c r="G18" s="141"/>
-      <c r="H18" s="141"/>
-      <c r="I18" s="141"/>
+      <c r="B18" s="142"/>
+      <c r="C18" s="142"/>
+      <c r="D18" s="142"/>
+      <c r="E18" s="142"/>
+      <c r="F18" s="142"/>
+      <c r="G18" s="142"/>
+      <c r="H18" s="142"/>
+      <c r="I18" s="142"/>
     </row>
     <row r="19" spans="1:26" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="93"/>
       <c r="B19" s="93"/>
-      <c r="C19" s="143" t="s">
+      <c r="C19" s="144" t="s">
         <v>413</v>
       </c>
-      <c r="D19" s="128"/>
-      <c r="E19" s="128"/>
-      <c r="F19" s="128"/>
-      <c r="G19" s="128"/>
-      <c r="H19" s="128"/>
-      <c r="I19" s="129"/>
+      <c r="D19" s="129"/>
+      <c r="E19" s="129"/>
+      <c r="F19" s="129"/>
+      <c r="G19" s="129"/>
+      <c r="H19" s="129"/>
+      <c r="I19" s="130"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="94"/>
       <c r="B20" s="95" t="s">
         <v>414</v>
       </c>
-      <c r="C20" s="144" t="s">
+      <c r="C20" s="145" t="s">
         <v>415</v>
       </c>
-      <c r="D20" s="145"/>
-      <c r="E20" s="145"/>
-      <c r="F20" s="146"/>
-      <c r="G20" s="144" t="s">
+      <c r="D20" s="146"/>
+      <c r="E20" s="146"/>
+      <c r="F20" s="147"/>
+      <c r="G20" s="145" t="s">
         <v>416</v>
       </c>
-      <c r="H20" s="145"/>
-      <c r="I20" s="146"/>
+      <c r="H20" s="146"/>
+      <c r="I20" s="147"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="96"/>
@@ -30070,7 +30070,7 @@
       </c>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="124" t="s">
+      <c r="A22" s="125" t="s">
         <v>418</v>
       </c>
       <c r="B22" s="101" t="s">
@@ -30087,7 +30087,7 @@
       <c r="I22" s="104"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="126"/>
+      <c r="A23" s="127"/>
       <c r="B23" s="106" t="s">
         <v>421</v>
       </c>
@@ -30112,7 +30112,7 @@
       </c>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="124" t="s">
+      <c r="A24" s="125" t="s">
         <v>426</v>
       </c>
       <c r="B24" s="101" t="s">
@@ -30141,7 +30141,7 @@
       </c>
     </row>
     <row r="25" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="125"/>
+      <c r="A25" s="126"/>
       <c r="B25" s="106" t="s">
         <v>431</v>
       </c>
@@ -30168,19 +30168,19 @@
       </c>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="126"/>
+      <c r="A26" s="127"/>
       <c r="B26" s="114" t="s">
         <v>434</v>
       </c>
-      <c r="C26" s="127" t="s">
+      <c r="C26" s="128" t="s">
         <v>435</v>
       </c>
-      <c r="D26" s="128"/>
-      <c r="E26" s="128"/>
-      <c r="F26" s="128"/>
-      <c r="G26" s="128"/>
-      <c r="H26" s="128"/>
-      <c r="I26" s="129"/>
+      <c r="D26" s="129"/>
+      <c r="E26" s="129"/>
+      <c r="F26" s="129"/>
+      <c r="G26" s="129"/>
+      <c r="H26" s="129"/>
+      <c r="I26" s="130"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="115" t="s">
@@ -30428,10 +30428,10 @@
       <c r="G44" s="122" t="s">
         <v>464</v>
       </c>
-      <c r="H44" s="130" t="s">
+      <c r="H44" s="131" t="s">
         <v>465</v>
       </c>
-      <c r="I44" s="131"/>
+      <c r="I44" s="132"/>
     </row>
     <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="67" t="s">
@@ -30446,8 +30446,8 @@
       <c r="G45" s="122" t="s">
         <v>467</v>
       </c>
-      <c r="H45" s="132"/>
-      <c r="I45" s="133"/>
+      <c r="H45" s="133"/>
+      <c r="I45" s="134"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="67" t="s">
@@ -30464,8 +30464,8 @@
       <c r="G46" s="123" t="s">
         <v>470</v>
       </c>
-      <c r="H46" s="134"/>
-      <c r="I46" s="135"/>
+      <c r="H46" s="135"/>
+      <c r="I46" s="136"/>
     </row>
     <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>